<commit_message>
Agregado pdf mejorado con tipo de pedido y verificar pedidos + ruleta
</commit_message>
<xml_diff>
--- a/porcentajes.xlsx
+++ b/porcentajes.xlsx
@@ -460,7 +460,7 @@
         <v>27</v>
       </c>
       <c r="C2" t="n">
-        <v>3.85</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="3">
@@ -473,98 +473,98 @@
         <v>19</v>
       </c>
       <c r="C3" t="n">
-        <v>2.71</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cecilia Gigena </t>
+          <t>Celia del Carmen Dibernardi</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C4" t="n">
-        <v>1.71</v>
+        <v>4.33</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Celia del Carmen Dibernardi</t>
+          <t xml:space="preserve">Cristina Lorente </t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C5" t="n">
-        <v>5.42</v>
+        <v>5.36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cristina Lorente </t>
+          <t>Florencia Marchese</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="C6" t="n">
-        <v>6.7</v>
+        <v>2.96</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Florencia Marchese</t>
+          <t>Leticia Ainsa</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C7" t="n">
-        <v>3.71</v>
+        <v>2.51</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Leticia Ainsa</t>
+          <t>Liliana Bennice</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="C8" t="n">
-        <v>3.14</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Liliana Bennice</t>
+          <t>MAGALI RIVAS</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="C9" t="n">
-        <v>9.130000000000001</v>
+        <v>4.1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MAGALI RIVAS</t>
+          <t>Magali Rivas</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C10" t="n">
-        <v>5.14</v>
+        <v>3.19</v>
       </c>
     </row>
     <row r="11">
@@ -574,23 +574,23 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="C11" t="n">
-        <v>9.99</v>
+        <v>11.86</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Marcia santa cruz</t>
+          <t>Maria Teresa Onega</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="C12" t="n">
-        <v>6.56</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="13">
@@ -603,7 +603,7 @@
         <v>57</v>
       </c>
       <c r="C13" t="n">
-        <v>8.130000000000001</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="14">
@@ -613,36 +613,36 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="C14" t="n">
-        <v>9.699999999999999</v>
+        <v>8.550000000000001</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Susana Lemmo</t>
+          <t>Silvia Pisellini Marchegiani</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>138</v>
+        <v>2</v>
       </c>
       <c r="C15" t="n">
-        <v>19.69</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Susana fernandez</t>
+          <t>Susana Lemmo</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>31</v>
+        <v>322</v>
       </c>
       <c r="C16" t="n">
-        <v>4.42</v>
+        <v>36.72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>